<commit_message>
update: agreement migration file new: trigger on update => record into log removed: log function update: now applications that need to have an action have different striped color update: tip-tool now have bigger font size update: 4 new status 91 executed agreement, 92 expired agreement, 100 imported executed agreement, 102 imported expired agreement new: mcom date counter function
</commit_message>
<xml_diff>
--- a/backend/uploads/moumoa.xlsx
+++ b/backend/uploads/moumoa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\moumoa\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1C24FF-8C6C-427F-BDDF-973CA2ABFA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C55A2F-F721-4800-B8C6-0C2CE534E55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A0D5F086-3978-4434-87A8-514A03AC8982}"/>
   </bookViews>
@@ -5273,15 +5273,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5810,8 +5802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A104FDD-41A4-4B8B-AE85-A9F07A0A6094}">
   <dimension ref="A1:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="J164" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L171" sqref="L171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5907,7 +5899,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M2" s="72">
         <v>81</v>
@@ -5946,7 +5938,7 @@
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M3" s="72"/>
     </row>
@@ -5985,7 +5977,7 @@
         <v>29</v>
       </c>
       <c r="L4" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M4" s="73"/>
     </row>
@@ -6024,7 +6016,7 @@
         <v>35</v>
       </c>
       <c r="L5" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M5" s="73"/>
     </row>
@@ -6063,7 +6055,7 @@
         <v>41</v>
       </c>
       <c r="L6" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M6" s="72"/>
     </row>
@@ -6102,7 +6094,7 @@
         <v>47</v>
       </c>
       <c r="L7" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M7" s="72"/>
     </row>
@@ -6141,7 +6133,7 @@
         <v>52</v>
       </c>
       <c r="L8" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M8" s="72"/>
     </row>
@@ -6180,7 +6172,7 @@
         <v>55</v>
       </c>
       <c r="L9" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M9" s="72"/>
     </row>
@@ -6219,7 +6211,7 @@
         <v>61</v>
       </c>
       <c r="L10" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M10" s="72"/>
     </row>
@@ -6258,7 +6250,7 @@
         <v>66</v>
       </c>
       <c r="L11" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M11" s="72"/>
     </row>
@@ -6297,7 +6289,7 @@
         <v>72</v>
       </c>
       <c r="L12" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M12" s="72"/>
     </row>
@@ -6336,7 +6328,7 @@
         <v>77</v>
       </c>
       <c r="L13" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M13" s="72"/>
     </row>
@@ -6375,7 +6367,7 @@
         <v>81</v>
       </c>
       <c r="L14" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M14" s="72"/>
     </row>
@@ -6414,7 +6406,7 @@
         <v>85</v>
       </c>
       <c r="L15" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M15" s="72"/>
     </row>
@@ -6453,7 +6445,7 @@
         <v>88</v>
       </c>
       <c r="L16" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M16" s="72"/>
     </row>
@@ -6492,7 +6484,7 @@
         <v>93</v>
       </c>
       <c r="L17" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M17" s="72"/>
     </row>
@@ -6531,7 +6523,7 @@
         <v>98</v>
       </c>
       <c r="L18" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M18" s="72"/>
     </row>
@@ -6570,7 +6562,7 @@
         <v>101</v>
       </c>
       <c r="L19" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M19" s="72"/>
     </row>
@@ -6609,7 +6601,7 @@
         <v>106</v>
       </c>
       <c r="L20" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M20" s="72"/>
     </row>
@@ -6646,7 +6638,7 @@
       </c>
       <c r="K21" s="52"/>
       <c r="L21" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M21" s="72"/>
     </row>
@@ -6685,7 +6677,7 @@
         <v>112</v>
       </c>
       <c r="L22" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M22" s="72"/>
     </row>
@@ -6724,7 +6716,7 @@
         <v>118</v>
       </c>
       <c r="L23" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M23" s="72"/>
     </row>
@@ -6763,7 +6755,7 @@
         <v>122</v>
       </c>
       <c r="L24" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M24" s="72"/>
     </row>
@@ -6802,7 +6794,7 @@
         <v>127</v>
       </c>
       <c r="L25" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M25" s="72"/>
     </row>
@@ -6841,11 +6833,11 @@
         <v>132</v>
       </c>
       <c r="L26" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M26" s="72"/>
     </row>
-    <row r="27" spans="1:13" ht="69" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>23</v>
       </c>
@@ -6880,7 +6872,7 @@
         <v>137</v>
       </c>
       <c r="L27" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M27" s="72"/>
     </row>
@@ -6919,7 +6911,7 @@
         <v>140</v>
       </c>
       <c r="L28" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M28" s="72"/>
     </row>
@@ -6958,7 +6950,7 @@
         <v>145</v>
       </c>
       <c r="L29" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M29" s="72"/>
     </row>
@@ -6997,7 +6989,7 @@
         <v>151</v>
       </c>
       <c r="L30" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M30" s="72"/>
     </row>
@@ -7036,7 +7028,7 @@
         <v>156</v>
       </c>
       <c r="L31" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M31" s="72"/>
     </row>
@@ -7075,7 +7067,7 @@
         <v>160</v>
       </c>
       <c r="L32" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M32" s="72"/>
     </row>
@@ -7112,7 +7104,7 @@
       </c>
       <c r="K33" s="52"/>
       <c r="L33" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M33" s="72"/>
     </row>
@@ -7151,7 +7143,7 @@
         <v>167</v>
       </c>
       <c r="L34" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M34" s="72"/>
     </row>
@@ -7190,7 +7182,7 @@
         <v>170</v>
       </c>
       <c r="L35" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M35" s="72"/>
     </row>
@@ -7229,7 +7221,7 @@
         <v>176</v>
       </c>
       <c r="L36" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M36" s="72"/>
     </row>
@@ -7268,7 +7260,7 @@
         <v>180</v>
       </c>
       <c r="L37" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M37" s="72"/>
     </row>
@@ -7305,7 +7297,7 @@
       </c>
       <c r="K38" s="52"/>
       <c r="L38" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M38" s="72"/>
     </row>
@@ -7344,7 +7336,7 @@
         <v>187</v>
       </c>
       <c r="L39" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M39" s="72"/>
     </row>
@@ -7383,7 +7375,7 @@
         <v>192</v>
       </c>
       <c r="L40" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M40" s="72"/>
     </row>
@@ -7422,7 +7414,7 @@
         <v>196</v>
       </c>
       <c r="L41" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M41" s="72"/>
     </row>
@@ -7461,7 +7453,7 @@
         <v>201</v>
       </c>
       <c r="L42" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M42" s="72"/>
     </row>
@@ -7500,7 +7492,7 @@
         <v>204</v>
       </c>
       <c r="L43" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M43" s="72"/>
     </row>
@@ -7539,7 +7531,7 @@
         <v>208</v>
       </c>
       <c r="L44" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M44" s="72"/>
     </row>
@@ -7578,7 +7570,7 @@
         <v>211</v>
       </c>
       <c r="L45" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M45" s="72"/>
     </row>
@@ -7617,7 +7609,7 @@
         <v>217</v>
       </c>
       <c r="L46" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M46" s="72"/>
     </row>
@@ -7656,7 +7648,7 @@
         <v>221</v>
       </c>
       <c r="L47" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M47" s="72"/>
     </row>
@@ -7695,7 +7687,7 @@
         <v>226</v>
       </c>
       <c r="L48" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M48" s="72"/>
     </row>
@@ -7734,7 +7726,7 @@
         <v>230</v>
       </c>
       <c r="L49" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M49" s="72"/>
     </row>
@@ -7773,7 +7765,7 @@
         <v>235</v>
       </c>
       <c r="L50" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M50" s="72"/>
     </row>
@@ -7812,7 +7804,7 @@
         <v>239</v>
       </c>
       <c r="L51" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M51" s="72"/>
     </row>
@@ -7851,7 +7843,7 @@
         <v>244</v>
       </c>
       <c r="L52" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M52" s="72"/>
     </row>
@@ -7890,7 +7882,7 @@
         <v>248</v>
       </c>
       <c r="L53" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M53" s="72"/>
     </row>
@@ -7929,7 +7921,7 @@
         <v>251</v>
       </c>
       <c r="L54" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M54" s="72"/>
     </row>
@@ -7968,7 +7960,7 @@
         <v>255</v>
       </c>
       <c r="L55" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M55" s="72"/>
     </row>
@@ -8005,7 +7997,7 @@
       </c>
       <c r="K56" s="53"/>
       <c r="L56" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="207" x14ac:dyDescent="0.25">
@@ -8043,7 +8035,7 @@
         <v>261</v>
       </c>
       <c r="L57" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M57" s="72"/>
     </row>
@@ -8082,7 +8074,7 @@
         <v>265</v>
       </c>
       <c r="L58" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M58" s="72"/>
     </row>
@@ -8121,7 +8113,7 @@
         <v>269</v>
       </c>
       <c r="L59" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M59" s="72"/>
     </row>
@@ -8160,7 +8152,7 @@
         <v>273</v>
       </c>
       <c r="L60" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M60" s="72"/>
     </row>
@@ -8199,7 +8191,7 @@
         <v>276</v>
       </c>
       <c r="L61" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M61" s="72"/>
     </row>
@@ -8238,7 +8230,7 @@
         <v>279</v>
       </c>
       <c r="L62" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M62" s="72"/>
     </row>
@@ -8277,7 +8269,7 @@
         <v>283</v>
       </c>
       <c r="L63" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M63" s="72"/>
     </row>
@@ -8316,7 +8308,7 @@
         <v>287</v>
       </c>
       <c r="L64" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M64" s="72"/>
     </row>
@@ -8355,7 +8347,7 @@
         <v>292</v>
       </c>
       <c r="L65" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M65" s="72"/>
     </row>
@@ -8394,7 +8386,7 @@
         <v>295</v>
       </c>
       <c r="L66" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M66" s="72"/>
     </row>
@@ -8433,7 +8425,7 @@
         <v>299</v>
       </c>
       <c r="L67" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M67" s="72"/>
     </row>
@@ -8472,7 +8464,7 @@
         <v>303</v>
       </c>
       <c r="L68" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M68" s="72"/>
     </row>
@@ -8511,7 +8503,7 @@
         <v>307</v>
       </c>
       <c r="L69" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M69" s="72"/>
     </row>
@@ -8550,7 +8542,7 @@
         <v>311</v>
       </c>
       <c r="L70" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M70" s="72"/>
     </row>
@@ -8589,7 +8581,7 @@
         <v>315</v>
       </c>
       <c r="L71" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M71" s="72"/>
     </row>
@@ -8628,7 +8620,7 @@
         <v>320</v>
       </c>
       <c r="L72" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M72" s="72"/>
     </row>
@@ -8667,7 +8659,7 @@
         <v>323</v>
       </c>
       <c r="L73" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M73" s="72"/>
     </row>
@@ -8706,7 +8698,7 @@
         <v>327</v>
       </c>
       <c r="L74" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M74" s="72"/>
     </row>
@@ -8745,7 +8737,7 @@
         <v>333</v>
       </c>
       <c r="L75" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M75" s="72"/>
     </row>
@@ -8784,11 +8776,11 @@
         <v>334</v>
       </c>
       <c r="L76" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M76" s="74"/>
     </row>
-    <row r="77" spans="1:13" ht="327.75" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" ht="345" x14ac:dyDescent="0.3">
       <c r="A77" s="9">
         <v>71</v>
       </c>
@@ -8823,7 +8815,7 @@
         <v>338</v>
       </c>
       <c r="L77" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M77" s="72"/>
     </row>
@@ -8862,7 +8854,7 @@
         <v>342</v>
       </c>
       <c r="L78" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M78" s="72"/>
     </row>
@@ -8901,7 +8893,7 @@
         <v>346</v>
       </c>
       <c r="L79" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M79" s="72"/>
     </row>
@@ -8940,7 +8932,7 @@
         <v>350</v>
       </c>
       <c r="L80" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M80" s="72"/>
     </row>
@@ -8979,7 +8971,7 @@
         <v>354</v>
       </c>
       <c r="L81" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M81" s="72"/>
     </row>
@@ -9018,7 +9010,7 @@
         <v>358</v>
       </c>
       <c r="L82" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M82" s="72"/>
     </row>
@@ -9057,7 +9049,7 @@
         <v>362</v>
       </c>
       <c r="L83" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M83" s="75"/>
     </row>
@@ -9096,7 +9088,7 @@
         <v>366</v>
       </c>
       <c r="L84" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M84" s="5"/>
     </row>
@@ -9135,7 +9127,7 @@
         <v>370</v>
       </c>
       <c r="L85" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M85" s="5"/>
     </row>
@@ -9174,7 +9166,7 @@
         <v>374</v>
       </c>
       <c r="L86" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M86" s="74"/>
     </row>
@@ -9213,7 +9205,7 @@
         <v>379</v>
       </c>
       <c r="L87" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M87" s="74"/>
     </row>
@@ -9252,7 +9244,7 @@
         <v>383</v>
       </c>
       <c r="L88" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M88" s="5"/>
     </row>
@@ -9291,7 +9283,7 @@
         <v>387</v>
       </c>
       <c r="L89" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M89" s="75"/>
     </row>
@@ -9330,7 +9322,7 @@
         <v>389</v>
       </c>
       <c r="L90" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M90" s="72"/>
     </row>
@@ -9369,7 +9361,7 @@
         <v>393</v>
       </c>
       <c r="L91" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M91" s="72"/>
     </row>
@@ -9408,7 +9400,7 @@
         <v>397</v>
       </c>
       <c r="L92" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M92" s="72"/>
     </row>
@@ -9447,7 +9439,7 @@
         <v>402</v>
       </c>
       <c r="L93" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M93" s="75"/>
     </row>
@@ -9486,7 +9478,7 @@
         <v>406</v>
       </c>
       <c r="L94" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M94" s="75"/>
     </row>
@@ -9525,7 +9517,7 @@
         <v>410</v>
       </c>
       <c r="L95" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M95" s="75"/>
     </row>
@@ -9564,7 +9556,7 @@
         <v>414</v>
       </c>
       <c r="L96" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M96" s="72"/>
     </row>
@@ -9603,7 +9595,7 @@
         <v>418</v>
       </c>
       <c r="L97" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M97" s="72"/>
     </row>
@@ -9642,7 +9634,7 @@
         <v>423</v>
       </c>
       <c r="L98" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M98" s="72"/>
     </row>
@@ -9681,7 +9673,7 @@
         <v>427</v>
       </c>
       <c r="L99" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M99" s="5"/>
     </row>
@@ -9720,7 +9712,7 @@
         <v>431</v>
       </c>
       <c r="L100" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M100" s="74"/>
     </row>
@@ -9759,7 +9751,7 @@
         <v>435</v>
       </c>
       <c r="L101" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M101" s="75"/>
     </row>
@@ -9798,7 +9790,7 @@
         <v>439</v>
       </c>
       <c r="L102" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M102" s="72"/>
     </row>
@@ -9837,7 +9829,7 @@
         <v>443</v>
       </c>
       <c r="L103" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M103" s="75"/>
     </row>
@@ -9876,7 +9868,7 @@
         <v>447</v>
       </c>
       <c r="L104" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M104" s="75"/>
     </row>
@@ -9915,7 +9907,7 @@
         <v>451</v>
       </c>
       <c r="L105" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M105" s="75"/>
     </row>
@@ -9954,7 +9946,7 @@
         <v>455</v>
       </c>
       <c r="L106" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M106" s="75"/>
     </row>
@@ -9993,7 +9985,7 @@
         <v>460</v>
       </c>
       <c r="L107" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M107" s="75"/>
     </row>
@@ -10032,7 +10024,7 @@
         <v>462</v>
       </c>
       <c r="L108" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M108" s="75"/>
     </row>
@@ -10071,7 +10063,7 @@
         <v>466</v>
       </c>
       <c r="L109" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M109" s="75"/>
     </row>
@@ -10110,7 +10102,7 @@
         <v>471</v>
       </c>
       <c r="L110" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M110" s="75"/>
     </row>
@@ -10149,7 +10141,7 @@
         <v>474</v>
       </c>
       <c r="L111" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M111" s="75"/>
     </row>
@@ -10188,7 +10180,7 @@
         <v>478</v>
       </c>
       <c r="L112" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M112" s="75"/>
     </row>
@@ -10227,7 +10219,7 @@
         <v>481</v>
       </c>
       <c r="L113" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M113" s="75"/>
     </row>
@@ -10266,7 +10258,7 @@
         <v>487</v>
       </c>
       <c r="L114" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M114" s="75"/>
     </row>
@@ -10305,7 +10297,7 @@
         <v>491</v>
       </c>
       <c r="L115" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M115" s="75"/>
     </row>
@@ -10344,7 +10336,7 @@
         <v>494</v>
       </c>
       <c r="L116" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M116" s="74"/>
     </row>
@@ -10383,7 +10375,7 @@
         <v>498</v>
       </c>
       <c r="L117" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M117" s="75"/>
     </row>
@@ -10422,7 +10414,7 @@
         <v>502</v>
       </c>
       <c r="L118" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M118" s="74"/>
     </row>
@@ -10461,7 +10453,7 @@
         <v>506</v>
       </c>
       <c r="L119" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M119" s="75"/>
     </row>
@@ -10500,7 +10492,7 @@
         <v>510</v>
       </c>
       <c r="L120" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M120" s="74"/>
     </row>
@@ -10539,7 +10531,7 @@
         <v>514</v>
       </c>
       <c r="L121" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M121" s="74"/>
     </row>
@@ -10578,7 +10570,7 @@
         <v>518</v>
       </c>
       <c r="L122" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M122" s="75"/>
     </row>
@@ -10617,7 +10609,7 @@
         <v>522</v>
       </c>
       <c r="L123" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M123" s="75"/>
     </row>
@@ -10656,7 +10648,7 @@
         <v>525</v>
       </c>
       <c r="L124" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M124" s="75"/>
     </row>
@@ -10695,7 +10687,7 @@
         <v>529</v>
       </c>
       <c r="L125" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M125" s="75"/>
     </row>
@@ -10734,7 +10726,7 @@
         <v>534</v>
       </c>
       <c r="L126" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M126" s="75"/>
     </row>
@@ -10773,7 +10765,7 @@
         <v>538</v>
       </c>
       <c r="L127" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M127" s="75"/>
     </row>
@@ -10812,7 +10804,7 @@
         <v>542</v>
       </c>
       <c r="L128" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M128" s="75"/>
     </row>
@@ -10851,7 +10843,7 @@
         <v>547</v>
       </c>
       <c r="L129" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M129" s="75"/>
     </row>
@@ -10890,7 +10882,7 @@
         <v>550</v>
       </c>
       <c r="L130" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M130" s="75"/>
     </row>
@@ -10929,7 +10921,7 @@
         <v>553</v>
       </c>
       <c r="L131" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M131" s="75"/>
     </row>
@@ -10968,7 +10960,7 @@
         <v>558</v>
       </c>
       <c r="L132" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M132" s="75"/>
     </row>
@@ -11007,7 +10999,7 @@
         <v>563</v>
       </c>
       <c r="L133" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M133" s="75"/>
     </row>
@@ -11042,7 +11034,7 @@
       <c r="J134" s="54"/>
       <c r="K134" s="54"/>
       <c r="L134" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M134" s="75"/>
     </row>
@@ -11081,7 +11073,7 @@
         <v>568</v>
       </c>
       <c r="L135" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M135" s="75"/>
     </row>
@@ -11120,7 +11112,7 @@
         <v>572</v>
       </c>
       <c r="L136" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M136" s="75"/>
     </row>
@@ -11159,7 +11151,7 @@
         <v>577</v>
       </c>
       <c r="L137" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M137" s="75"/>
     </row>
@@ -11198,7 +11190,7 @@
         <v>583</v>
       </c>
       <c r="L138" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M138" s="75"/>
     </row>
@@ -11233,7 +11225,7 @@
       <c r="J139" s="55"/>
       <c r="K139" s="55"/>
       <c r="L139" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M139" s="76"/>
     </row>
@@ -11272,7 +11264,7 @@
         <v>589</v>
       </c>
       <c r="L140" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M140" s="75"/>
     </row>
@@ -11311,7 +11303,7 @@
         <v>593</v>
       </c>
       <c r="L141" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M141" s="75"/>
     </row>
@@ -11350,7 +11342,7 @@
         <v>597</v>
       </c>
       <c r="L142" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M142" s="75"/>
     </row>
@@ -11389,7 +11381,7 @@
         <v>601</v>
       </c>
       <c r="L143" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M143" s="75"/>
     </row>
@@ -11428,7 +11420,7 @@
         <v>604</v>
       </c>
       <c r="L144" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M144" s="77"/>
     </row>
@@ -11467,7 +11459,7 @@
         <v>607</v>
       </c>
       <c r="L145" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M145" s="77"/>
     </row>
@@ -11506,7 +11498,7 @@
         <v>612</v>
       </c>
       <c r="L146" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="147" spans="1:13" ht="34.5" x14ac:dyDescent="0.25">
@@ -11538,7 +11530,7 @@
       <c r="J147" s="56"/>
       <c r="K147" s="56"/>
       <c r="L147" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="148" spans="1:13" ht="103.5" x14ac:dyDescent="0.25">
@@ -11576,7 +11568,7 @@
         <v>615</v>
       </c>
       <c r="L148" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
@@ -11614,7 +11606,7 @@
         <v>619</v>
       </c>
       <c r="L149" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="150" spans="1:13" ht="155.25" x14ac:dyDescent="0.25">
@@ -11652,7 +11644,7 @@
         <v>623</v>
       </c>
       <c r="L150" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M150" s="78"/>
     </row>
@@ -11691,7 +11683,7 @@
         <v>625</v>
       </c>
       <c r="L151" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M151" s="75"/>
     </row>
@@ -11730,7 +11722,7 @@
         <v>630</v>
       </c>
       <c r="L152" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="153" spans="1:13" ht="224.25" x14ac:dyDescent="0.25">
@@ -11768,7 +11760,7 @@
         <v>634</v>
       </c>
       <c r="L153" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M153" s="76"/>
     </row>
@@ -11807,7 +11799,7 @@
         <v>639</v>
       </c>
       <c r="L154" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="155" spans="1:13" ht="155.25" x14ac:dyDescent="0.25">
@@ -11843,7 +11835,7 @@
       </c>
       <c r="K155" s="56"/>
       <c r="L155" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="156" spans="1:13" ht="86.25" x14ac:dyDescent="0.25">
@@ -11879,7 +11871,7 @@
       </c>
       <c r="K156" s="56"/>
       <c r="L156" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="157" spans="1:13" ht="155.25" x14ac:dyDescent="0.25">
@@ -11915,7 +11907,7 @@
       </c>
       <c r="K157" s="57"/>
       <c r="L157" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M157" s="78"/>
     </row>
@@ -11952,7 +11944,7 @@
       </c>
       <c r="K158" s="12"/>
       <c r="L158" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M158" s="76"/>
     </row>
@@ -11985,7 +11977,7 @@
       <c r="J159" s="58"/>
       <c r="K159" s="58"/>
       <c r="L159" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="160" spans="1:13" ht="103.5" x14ac:dyDescent="0.25">
@@ -12023,7 +12015,7 @@
         <v>657</v>
       </c>
       <c r="L160" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="161" spans="1:13" ht="103.5" x14ac:dyDescent="0.25">
@@ -12061,7 +12053,7 @@
         <v>660</v>
       </c>
       <c r="L161" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="162" spans="1:13" ht="224.25" x14ac:dyDescent="0.25">
@@ -12095,7 +12087,7 @@
       <c r="J162" s="56"/>
       <c r="K162" s="56"/>
       <c r="L162" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="163" spans="1:13" ht="155.25" x14ac:dyDescent="0.3">
@@ -12129,7 +12121,7 @@
       <c r="J163" s="42"/>
       <c r="K163" s="42"/>
       <c r="L163" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M163" s="80"/>
     </row>
@@ -12164,7 +12156,7 @@
       <c r="J164" s="12"/>
       <c r="K164" s="12"/>
       <c r="L164" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M164" s="76"/>
     </row>
@@ -12199,7 +12191,7 @@
       <c r="J165" s="12"/>
       <c r="K165" s="12"/>
       <c r="L165" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M165" s="76"/>
     </row>
@@ -12234,7 +12226,7 @@
       <c r="J166" s="12"/>
       <c r="K166" s="12"/>
       <c r="L166" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M166" s="76"/>
     </row>
@@ -12269,7 +12261,7 @@
       <c r="J167" s="12"/>
       <c r="K167" s="12"/>
       <c r="L167" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="M167" s="76"/>
     </row>
@@ -12286,7 +12278,7 @@
       <c r="J168" s="70"/>
       <c r="K168" s="70"/>
       <c r="L168" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="169" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
@@ -12302,7 +12294,7 @@
       <c r="J169" s="70"/>
       <c r="K169" s="70"/>
       <c r="L169" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="170" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
@@ -12318,7 +12310,7 @@
       <c r="J170" s="70"/>
       <c r="K170" s="70"/>
       <c r="L170" s="72">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="171" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">

</xml_diff>